<commit_message>
HS 7 Y 8
</commit_message>
<xml_diff>
--- a/Documentacion_Proyecto/Desarrollo Movil - Historias de usuario.xlsx
+++ b/Documentacion_Proyecto/Desarrollo Movil - Historias de usuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\600ESAN\9SEMESTRE\DAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean Pierre\Desktop\MOVILES\Proyecto_Final\Documentacion_Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361C0F39-6F4F-4790-9048-AF6CC3079456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F251C7D2-9D7B-40B7-ADC5-20540C31068B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalles de Usuario" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="110">
   <si>
     <t xml:space="preserve">N° </t>
   </si>
@@ -195,15 +195,9 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Como cliente, deseo acceder a las mejores pasarelas de pago disponibles en el sistema, con el fin de realizar reservas de manera rápida, segura y sin inconvenientes.</t>
-  </si>
-  <si>
     <t>Como empresa turística, deseo tener acceso al historial completo de actividades de mis clientes en el sistema, con el fin de identificar a los clientes frecuentes y ofrecerles ofertas personalizadas y beneficios especiales</t>
   </si>
   <si>
-    <t>El sistema muestra opciones de pasarelas de pago reconocidas y confiables al momento de realizar una reserva</t>
-  </si>
-  <si>
     <t>El sistema proporciona un panel o sección específica para que la empresa turística acceda al historial de actividades de sus clientes</t>
   </si>
   <si>
@@ -346,6 +340,18 @@
   </si>
   <si>
     <t>La empresa turística debe ingresar datos como Nombre de la empresa, Email corporativo, Contraseña, Celular, Ruc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opciones de pagos </t>
+  </si>
+  <si>
+    <t>Como cliente, deseo tener diferentes formas de pago disponibles en el sistema, con el fin de realizar reservas de manera rápida, segura y sin inconvenientes.</t>
+  </si>
+  <si>
+    <t>El sistema muestra opciones de pago reconocidas y confiables al momento de realizar una reserva</t>
+  </si>
+  <si>
+    <t>Los clientes podran acceder a esta seccion desde Reservar Actividad</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -550,21 +556,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -787,19 +796,19 @@
   </sheetPr>
   <dimension ref="C2:H101"/>
   <sheetViews>
-    <sheetView topLeftCell="C58" workbookViewId="0">
-      <selection activeCell="G61" sqref="G53:H61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78:D78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1"/>
-    <col min="8" max="8" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -827,7 +836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
@@ -841,7 +850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
@@ -855,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
@@ -869,7 +878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
@@ -883,81 +892,81 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C8" s="18" t="s">
+    <row r="8" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="G8" s="18" t="s">
+      <c r="D8" s="20"/>
+      <c r="G8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="20" t="s">
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="17"/>
       <c r="G9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="24"/>
-    </row>
-    <row r="10" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C10" s="20" t="s">
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C11" s="20" t="s">
+    <row r="11" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C12" s="20" t="s">
+    <row r="12" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C12" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C13" s="16"/>
+    <row r="13" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C13" s="18"/>
       <c r="D13" s="17"/>
-      <c r="G13" s="16"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="17"/>
     </row>
-    <row r="14" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C14" s="16"/>
+    <row r="14" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C14" s="18"/>
       <c r="D14" s="17"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C15" s="16"/>
+    <row r="15" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C15" s="18"/>
       <c r="D15" s="17"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C16" s="16"/>
+    <row r="16" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C16" s="18"/>
       <c r="D16" s="17"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="19" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
@@ -971,7 +980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
@@ -985,7 +994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>11</v>
       </c>
@@ -1024,10 +1033,10 @@
         <v>11</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="38.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>14</v>
       </c>
@@ -1041,81 +1050,81 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C25" s="18" t="s">
+    <row r="25" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="G25" s="18" t="s">
+      <c r="D25" s="20"/>
+      <c r="G25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="G26" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="G26" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C27" s="20" t="s">
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C27" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="17"/>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="16" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="G28" s="20" t="s">
-        <v>106</v>
+      <c r="D28" s="22"/>
+      <c r="G28" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C29" s="20" t="s">
+    <row r="29" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C29" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="17"/>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C30" s="16"/>
+    <row r="30" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C30" s="18"/>
       <c r="D30" s="17"/>
-      <c r="G30" s="16"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C31" s="16"/>
+    <row r="31" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C31" s="18"/>
       <c r="D31" s="17"/>
-      <c r="G31" s="16"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="16"/>
+    <row r="32" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C32" s="18"/>
       <c r="D32" s="17"/>
-      <c r="G32" s="16"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="16"/>
+    <row r="33" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C33" s="18"/>
       <c r="D33" s="17"/>
-      <c r="G33" s="16"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="17"/>
     </row>
-    <row r="36" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
         <v>11</v>
       </c>
@@ -1182,10 +1191,10 @@
         <v>11</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" ht="51" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="C41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1199,79 +1208,79 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C42" s="18" t="s">
+    <row r="42" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="G42" s="18" t="s">
+      <c r="D42" s="20"/>
+      <c r="G42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="19"/>
-    </row>
-    <row r="43" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C43" s="20" t="s">
+      <c r="H42" s="20"/>
+    </row>
+    <row r="43" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C43" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="17"/>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="16" t="s">
         <v>46</v>
       </c>
       <c r="H43" s="17"/>
     </row>
-    <row r="44" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="21" t="s">
         <v>47</v>
       </c>
       <c r="D44" s="17"/>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="16" t="s">
         <v>48</v>
       </c>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C45" s="20" t="s">
+    <row r="45" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C45" s="16" t="s">
         <v>49</v>
       </c>
       <c r="D45" s="17"/>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="16" t="s">
         <v>50</v>
       </c>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C46" s="20" t="s">
+    <row r="46" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C46" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D46" s="17"/>
-      <c r="G46" s="20"/>
+      <c r="G46" s="16"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C47" s="16"/>
+    <row r="47" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C47" s="18"/>
       <c r="D47" s="17"/>
-      <c r="G47" s="16"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C48" s="16"/>
+    <row r="48" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C48" s="18"/>
       <c r="D48" s="17"/>
-      <c r="G48" s="16"/>
+      <c r="G48" s="18"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C49" s="16"/>
+    <row r="49" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C49" s="18"/>
       <c r="D49" s="17"/>
-      <c r="G49" s="16"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C50" s="16"/>
+    <row r="50" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C50" s="18"/>
       <c r="D50" s="17"/>
-      <c r="G50" s="16"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="53" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>24</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
@@ -1299,12 +1308,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C55" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>6</v>
@@ -1313,7 +1322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C57" s="3" t="s">
         <v>11</v>
       </c>
@@ -1341,91 +1350,93 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="3:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:8" ht="66" x14ac:dyDescent="0.25">
       <c r="C58" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C59" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C59" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="19"/>
-      <c r="G59" s="18" t="s">
+      <c r="D59" s="20"/>
+      <c r="G59" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="19"/>
-    </row>
-    <row r="60" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H59" s="20"/>
+    </row>
+    <row r="60" spans="3:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="21" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="D60" s="17"/>
       <c r="G60" s="21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H60" s="17"/>
     </row>
-    <row r="61" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="21" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="D61" s="17"/>
       <c r="G61" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H61" s="17"/>
     </row>
-    <row r="62" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C62" s="20"/>
+    <row r="62" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C62" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="D62" s="17"/>
-      <c r="G62" s="20"/>
+      <c r="G62" s="16"/>
       <c r="H62" s="17"/>
     </row>
-    <row r="63" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C63" s="20"/>
+    <row r="63" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C63" s="16"/>
       <c r="D63" s="17"/>
     </row>
-    <row r="64" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C64" s="16"/>
+    <row r="64" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C64" s="18"/>
       <c r="D64" s="17"/>
     </row>
-    <row r="65" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C65" s="16"/>
+    <row r="65" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C65" s="18"/>
       <c r="D65" s="17"/>
     </row>
-    <row r="66" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C66" s="16"/>
+    <row r="66" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C66" s="18"/>
       <c r="D66" s="17"/>
     </row>
-    <row r="67" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C67" s="16"/>
+    <row r="67" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C67" s="18"/>
       <c r="D67" s="17"/>
     </row>
-    <row r="70" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C71" s="3" t="s">
         <v>3</v>
       </c>
@@ -1439,21 +1450,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C72" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="73" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C73" s="3" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C74" s="3" t="s">
         <v>11</v>
       </c>
@@ -1481,83 +1492,83 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="3:8" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:8" ht="66" x14ac:dyDescent="0.25">
       <c r="C75" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H75" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C76" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="20"/>
+      <c r="G76" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="20"/>
+    </row>
+    <row r="77" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="G77" s="21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="76" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C76" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="19"/>
-      <c r="G76" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H76" s="19"/>
-    </row>
-    <row r="77" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C77" s="21" t="s">
+      <c r="H77" s="17"/>
+    </row>
+    <row r="78" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D77" s="17"/>
-      <c r="G77" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="H77" s="17"/>
-    </row>
-    <row r="78" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78" s="17"/>
+      <c r="D78" s="25"/>
       <c r="G78" s="21"/>
       <c r="H78" s="17"/>
     </row>
-    <row r="79" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C79" s="20"/>
-      <c r="D79" s="17"/>
-      <c r="G79" s="20"/>
+    <row r="79" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C79" s="21"/>
+      <c r="D79" s="25"/>
+      <c r="G79" s="16"/>
       <c r="H79" s="17"/>
     </row>
-    <row r="80" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C80" s="20"/>
+    <row r="80" spans="3:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C80" s="16"/>
       <c r="D80" s="17"/>
     </row>
-    <row r="81" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C81" s="16"/>
+    <row r="81" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C81" s="18"/>
       <c r="D81" s="17"/>
     </row>
-    <row r="82" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C82" s="16"/>
+    <row r="82" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C82" s="18"/>
       <c r="D82" s="17"/>
     </row>
-    <row r="83" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C83" s="16"/>
+    <row r="83" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C83" s="18"/>
       <c r="D83" s="17"/>
     </row>
-    <row r="84" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C84" s="16"/>
+    <row r="84" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C84" s="18"/>
       <c r="D84" s="17"/>
     </row>
-    <row r="87" spans="3:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" ht="15" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C88" s="3" t="s">
         <v>3</v>
       </c>
@@ -1565,15 +1576,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="3:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C89" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="90" spans="3:4" ht="15" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C90" s="3" t="s">
         <v>9</v>
       </c>
@@ -1581,79 +1592,115 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="3:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C91" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="3:4" ht="63.75" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" ht="66" x14ac:dyDescent="0.25">
       <c r="C92" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="93" spans="3:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="C93" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C93" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="19"/>
-    </row>
-    <row r="94" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D93" s="20"/>
+    </row>
+    <row r="94" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D94" s="24"/>
-    </row>
-    <row r="95" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="D94" s="22"/>
+    </row>
+    <row r="95" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C95" s="21"/>
       <c r="D95" s="17"/>
     </row>
-    <row r="96" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C96" s="20"/>
+    <row r="96" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C96" s="16"/>
       <c r="D96" s="17"/>
     </row>
-    <row r="97" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C97" s="20"/>
+    <row r="97" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C97" s="16"/>
       <c r="D97" s="17"/>
     </row>
-    <row r="98" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C98" s="16"/>
+    <row r="98" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C98" s="18"/>
       <c r="D98" s="17"/>
     </row>
-    <row r="99" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C99" s="16"/>
+    <row r="99" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C99" s="18"/>
       <c r="D99" s="17"/>
     </row>
-    <row r="100" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C100" s="16"/>
+    <row r="100" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C100" s="18"/>
       <c r="D100" s="17"/>
     </row>
-    <row r="101" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C101" s="16"/>
+    <row r="101" spans="3:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C101" s="18"/>
       <c r="D101" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -1663,53 +1710,19 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="G62:H62"/>
     <mergeCell ref="G60:H60"/>
     <mergeCell ref="G61:H61"/>
     <mergeCell ref="C48:D48"/>
@@ -1721,13 +1734,11 @@
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="G49:H49"/>
     <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1740,31 +1751,31 @@
   </sheetPr>
   <dimension ref="B3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>26</v>
       </c>
@@ -1792,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1820,7 +1831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>39</v>
       </c>
@@ -1834,7 +1845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>40</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
@@ -1862,12 +1873,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>13</v>
@@ -1876,12 +1887,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>31</v>
@@ -1890,7 +1901,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>53</v>
       </c>
@@ -1904,12 +1915,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>30</v>
@@ -1932,161 +1943,161 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C2" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="3:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="3:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="10" t="s">
+    </row>
+    <row r="4" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="D4" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>88</v>
-      </c>
       <c r="F4" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C5" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C6" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C9" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C10" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G14" s="5"/>
     </row>
   </sheetData>

</xml_diff>